<commit_message>
excel 2 rows changes
</commit_message>
<xml_diff>
--- a/try  my exel.xlsx
+++ b/try  my exel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>MANAGER</t>
   </si>
@@ -25,29 +25,10 @@
     <t>UI</t>
   </si>
   <si>
-    <t>Low/Minor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Summary:
-"DEMOABHYAS - UNIQVAL DEMO INSTANCE" should be enlarged 
-Steps to Reproduce:
-Step 1. Login as Manager
-Observation: 
-Since it is the opening page of the application the look and feel of the application improvises by enlargning the size of  "DEMOABHYAS - UNIQVAL DEMO INSTANCE" </t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
     <t>High/Major</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summary:
-"Menu drop-down closes the abhyaspod logo.
-Steps to Reproduce:
-Step 1. Login as Manager
-Observation: 
-When we click on Menu dropdown it hides the abhyaspod logo also with navigation panel,logo should not be hidden it should be same. </t>
   </si>
   <si>
     <t xml:space="preserve">Summary:
@@ -554,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,59 +544,31 @@
     <col min="6" max="6" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="H1" s="8"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>7</v>
-      </c>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -629,19 +582,19 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -655,51 +608,19 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4">
-      <formula1>"New,Open/Reopen, Assigned, In Progress, Verified/Closed, Not a defect, Duplicate, Fixed"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E4">
-      <formula1>"Blocker/Show Stopper/Critical, High/Major,Medium,Low/Minor,Cosmetic"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[1]TEST DATA'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1:C4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[1]TEST DATA'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'[1]TEST DATA'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:D4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>